<commit_message>
Indexed new color page in manual and spreadsheet
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2019fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2019fall.xlsx
@@ -2009,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2843,6 +2843,9 @@
       <c r="C17" s="14">
         <v>5</v>
       </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
       <c r="E17" s="14">
         <v>9</v>
       </c>
@@ -3112,16 +3115,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W23,C$2:C$72)</f>
+        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$72,"&gt;=" &amp; W23,C$2:C$72)</f>
         <v>304</v>
       </c>
       <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W23,D$2:D$72)</f>
-        <v>7</v>
+        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$72,"&gt;=" &amp; W23,D$2:D$72)</f>
+        <v>8</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>26.390000000000008</v>
+        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <v>26.78</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3188,16 +3191,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W24,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>274</v>
       </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W24,D$2:D$72)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Z24" s="8">
-        <f t="shared" si="1"/>
-        <v>24.050000000000004</v>
+        <f t="shared" si="3"/>
+        <v>24.440000000000005</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3248,16 +3251,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W25,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>234</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W25,D$2:D$72)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Z25" s="8">
-        <f t="shared" si="1"/>
-        <v>21.45</v>
+        <f t="shared" si="3"/>
+        <v>21.840000000000003</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3318,16 +3321,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W26,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W26,D$2:D$72)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="1"/>
-        <v>20.540000000000003</v>
+        <f t="shared" si="3"/>
+        <v>20.930000000000003</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3396,16 +3399,16 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W27,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>203</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W27,D$2:D$72)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Z27" s="8">
-        <f t="shared" si="1"/>
-        <v>19.434999999999999</v>
+        <f t="shared" si="3"/>
+        <v>19.824999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3459,16 +3462,16 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W28,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>159</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W28,D$2:D$72)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="1"/>
-        <v>16.574999999999999</v>
+        <f t="shared" si="3"/>
+        <v>16.965</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -3501,15 +3504,15 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W29,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W29,D$2:D$72)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15.795000000000003</v>
       </c>
     </row>
@@ -3562,15 +3565,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W30,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W30,D$2:D$72)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3631,15 +3634,15 @@
         <v>4</v>
       </c>
       <c r="X31" s="47">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W31,C$2:C$72)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$72,"&gt;=" &amp; W31,D$2:D$72)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z31" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -5379,7 +5382,7 @@
       </c>
       <c r="T68" s="34"/>
       <c r="U68" s="77">
-        <f t="shared" ref="U68:U71" si="2">SUM(Q68:T68)</f>
+        <f t="shared" ref="U68:U71" si="4">SUM(Q68:T68)</f>
         <v>1</v>
       </c>
       <c r="V68" s="15"/>
@@ -5425,7 +5428,7 @@
       </c>
       <c r="T69" s="34"/>
       <c r="U69" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V69" s="15"/>
@@ -5471,7 +5474,7 @@
       </c>
       <c r="T70" s="34"/>
       <c r="U70" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V70" s="15"/>
@@ -5516,7 +5519,7 @@
       </c>
       <c r="T71" s="37"/>
       <c r="U71" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V71" s="15"/>
@@ -5636,15 +5639,15 @@
       <c r="O76" s="68"/>
       <c r="P76" s="68"/>
       <c r="Q76" s="68">
-        <f t="shared" ref="Q76:S76" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <f t="shared" ref="Q76:S76" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
         <v>234</v>
       </c>
       <c r="R76" s="68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="S76" s="68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="T76" s="69"/>
@@ -5671,15 +5674,15 @@
       <c r="O77" s="70"/>
       <c r="P77" s="70"/>
       <c r="Q77" s="70">
-        <f t="shared" ref="Q77:S77" si="4">Q74/Q76</f>
+        <f t="shared" ref="Q77:S77" si="6">Q74/Q76</f>
         <v>0.81623931623931623</v>
       </c>
       <c r="R77" s="70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.9128205128205128</v>
       </c>
       <c r="S77" s="70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.87790598290598298</v>
       </c>
       <c r="T77" s="71"/>
@@ -5702,15 +5705,15 @@
       <c r="O78" s="73"/>
       <c r="P78" s="73"/>
       <c r="Q78" s="73">
-        <f t="shared" ref="Q78:S78" si="5">Q76-Q74</f>
+        <f t="shared" ref="Q78:S78" si="7">Q76-Q74</f>
         <v>43</v>
       </c>
       <c r="R78" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20.400000000000006</v>
       </c>
       <c r="S78" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28.569999999999993</v>
       </c>
       <c r="T78" s="74"/>

</xml_diff>

<commit_message>
updated color page indexing, page counts in spreadsheet
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2019fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2019fall.xlsx
@@ -2009,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2841,7 +2841,7 @@
         <v>130</v>
       </c>
       <c r="C17" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="14">
         <v>1</v>
@@ -3116,15 +3116,15 @@
       </c>
       <c r="X23" s="6">
         <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$72,"&gt;=" &amp; W23,C$2:C$72)</f>
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="Y23" s="6">
         <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$72,"&gt;=" &amp; W23,D$2:D$72)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>26.78</v>
+        <v>28.080000000000002</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3192,15 +3192,15 @@
       </c>
       <c r="X24" s="6">
         <f t="shared" si="1"/>
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="Y24" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="3"/>
-        <v>24.440000000000005</v>
+        <v>25.740000000000002</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3252,15 +3252,15 @@
       </c>
       <c r="X25" s="6">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="Y25" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="3"/>
-        <v>21.840000000000003</v>
+        <v>23.14</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3322,15 +3322,15 @@
       </c>
       <c r="X26" s="31">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="Y26" s="31">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>20.930000000000003</v>
+        <v>22.230000000000004</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3400,15 +3400,15 @@
       </c>
       <c r="X27" s="6">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="3"/>
-        <v>19.824999999999999</v>
+        <v>21.125</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3463,15 +3463,15 @@
       </c>
       <c r="X28" s="6">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
-        <v>16.965</v>
+        <v>18.265000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -3505,15 +3505,15 @@
       </c>
       <c r="X29" s="6">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Y29" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="3"/>
-        <v>15.795000000000003</v>
+        <v>17.03</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -3965,9 +3965,11 @@
         <v>151</v>
       </c>
       <c r="C39" s="13">
-        <v>6</v>
-      </c>
-      <c r="D39" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="D39" s="13">
+        <v>2</v>
+      </c>
       <c r="E39" s="13">
         <v>21</v>
       </c>
@@ -4023,6 +4025,9 @@
       </c>
       <c r="C40" s="14">
         <v>6</v>
+      </c>
+      <c r="D40" s="14">
+        <v>1</v>
       </c>
       <c r="E40" s="14">
         <v>22</v>
@@ -5549,15 +5554,15 @@
       <c r="P73" s="65"/>
       <c r="Q73" s="65">
         <f t="array" ref="Q73">SUM($C2:$C71*(Q2:Q71&gt;=0.9)*($U2:$U71&gt;=$W$12))</f>
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="R73" s="65">
         <f t="array" ref="R73">SUM($C2:$C71*(R2:R71&gt;=0.9)*($U2:$U71&gt;=$W$12))</f>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="S73" s="65">
         <f t="array" ref="S73">SUM($C2:$C71*(S2:S71&gt;=0.9)*($U2:$U71&gt;=$W$12))</f>
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T73" s="66"/>
       <c r="V73" s="15"/>
@@ -5576,15 +5581,15 @@
       <c r="P74" s="68"/>
       <c r="Q74" s="68">
         <f t="array" ref="Q74">SUM($C2:$C71*Q2:Q71*($U2:$U71&gt;=$W$12))</f>
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="R74" s="68">
         <f t="array" ref="R74">SUM($C2:$C71*R2:R71*($U2:$U71&gt;=$W$12))</f>
-        <v>213.6</v>
+        <v>215.6</v>
       </c>
       <c r="S74" s="68">
         <f t="array" ref="S74">SUM($C2:$C71*S2:S71*($U2:$U71&gt;=$W$12))</f>
-        <v>205.43</v>
+        <v>207.23</v>
       </c>
       <c r="T74" s="69"/>
       <c r="V74" s="15"/>
@@ -5606,15 +5611,15 @@
       <c r="P75" s="68"/>
       <c r="Q75" s="68">
         <f t="array" ref="Q75">SUM($C$2:$C$71*(Q$2:Q$71&gt;=0.1)*($U$2:$U$71&gt;=$W$12))</f>
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="R75" s="68">
         <f t="array" ref="R75">SUM($C$2:$C$71*(R$2:R$71&gt;=0.1)*($U$2:$U$71&gt;=$W$12))</f>
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="S75" s="68">
         <f t="array" ref="S75">SUM($C$2:$C$71*(S$2:S$71&gt;=0.1)*($U$2:$U$71&gt;=$W$12))</f>
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="T75" s="69"/>
       <c r="V75" s="15"/>
@@ -5640,15 +5645,15 @@
       <c r="P76" s="68"/>
       <c r="Q76" s="68">
         <f t="shared" ref="Q76:S76" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="R76" s="68">
         <f t="shared" si="5"/>
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="S76" s="68">
         <f t="shared" si="5"/>
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="T76" s="69"/>
       <c r="U76" s="3"/>
@@ -5675,15 +5680,15 @@
       <c r="P77" s="70"/>
       <c r="Q77" s="70">
         <f t="shared" ref="Q77:S77" si="6">Q74/Q76</f>
-        <v>0.81623931623931623</v>
+        <v>0.81779661016949157</v>
       </c>
       <c r="R77" s="70">
         <f t="shared" si="6"/>
-        <v>0.9128205128205128</v>
+        <v>0.91355932203389834</v>
       </c>
       <c r="S77" s="70">
         <f t="shared" si="6"/>
-        <v>0.87790598290598298</v>
+        <v>0.87809322033898296</v>
       </c>
       <c r="T77" s="71"/>
       <c r="V77" s="15"/>
@@ -5714,7 +5719,7 @@
       </c>
       <c r="S78" s="73">
         <f t="shared" si="7"/>
-        <v>28.569999999999993</v>
+        <v>28.77000000000001</v>
       </c>
       <c r="T78" s="74"/>
       <c r="V78" s="15"/>

</xml_diff>